<commit_message>
Made changes to Benefits in Policy Modal
</commit_message>
<xml_diff>
--- a/paramData Excels/P0027.xlsx
+++ b/paramData Excels/P0027.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>COLUMN_KEY</t>
   </si>
@@ -171,6 +171,24 @@
   </si>
   <si>
     <t>GlSign</t>
+  </si>
+  <si>
+    <t>Help_text</t>
+  </si>
+  <si>
+    <t>help_desc</t>
+  </si>
+  <si>
+    <t>The generic Account code is defined for each entry</t>
+  </si>
+  <si>
+    <t>This field denotes the sequence number assigned to an accounting entry in a transaction.</t>
+  </si>
+  <si>
+    <t>This column represents whether the mentioned Account code has to be debited (+) or credited (-). Both credit and debit amounts for any financial ransaction should tally.</t>
+  </si>
+  <si>
+    <t>The Accounting rules for all financial transaction codes  need to be configured in this table; these rules  are referred to at the time of processing the respective transactions. Multiple accounting entries could be defined for each transction code. The impacted e Account codes, sequence number and credit(-)/debit(+) details are need to be configured for each entry.</t>
   </si>
 </sst>
 </file>
@@ -213,7 +231,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +268,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -263,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -272,6 +296,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,9 +620,10 @@
     <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.5703125" customWidth="1"/>
     <col min="19" max="19" width="9.42578125" customWidth="1"/>
+    <col min="26" max="26" width="89.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,8 +685,14 @@
         <v>16</v>
       </c>
       <c r="U1" s="6"/>
+      <c r="Z1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>31</v>
       </c>
@@ -694,8 +726,14 @@
       <c r="T2">
         <v>1</v>
       </c>
+      <c r="Z2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>2</v>
       </c>
@@ -724,7 +762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>3</v>
       </c>
@@ -752,8 +790,11 @@
       <c r="T4">
         <v>3</v>
       </c>
+      <c r="Z4" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>4</v>
       </c>
@@ -783,6 +824,9 @@
       </c>
       <c r="T5">
         <v>4</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Enquiry to remaining Params
</commit_message>
<xml_diff>
--- a/paramData Excels/P0027.xlsx
+++ b/paramData Excels/P0027.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AD80D32-AE3B-4CCF-B4A4-1FC5B028D267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +15,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -43,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>COLUMN_KEY</t>
   </si>
@@ -173,29 +174,26 @@
     <t>GlSign</t>
   </si>
   <si>
-    <t>Help_text</t>
-  </si>
-  <si>
-    <t>help_desc</t>
-  </si>
-  <si>
-    <t>The generic Account code is defined for each entry</t>
-  </si>
-  <si>
-    <t>This field denotes the sequence number assigned to an accounting entry in a transaction.</t>
-  </si>
-  <si>
-    <t>This column represents whether the mentioned Account code has to be debited (+) or credited (-). Both credit and debit amounts for any financial ransaction should tally.</t>
-  </si>
-  <si>
-    <t>The Accounting rules for all financial transaction codes  need to be configured in this table; these rules  are referred to at the time of processing the respective transactions. Multiple accounting entries could be defined for each transction code. The impacted e Account codes, sequence number and credit(-)/debit(+) details are need to be configured for each entry.</t>
+    <t>Provides the Accounting Codes used by Finance &amp; Accounts Department</t>
+  </si>
+  <si>
+    <t>Accounting movements having financial implications on the contract</t>
+  </si>
+  <si>
+    <t>Amount as per the transactions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seqence Number </t>
+  </si>
+  <si>
+    <t>Group Ledger Sign (Debit or Credit)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,8 +228,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,19 +273,28 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -296,7 +310,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -315,9 +331,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -355,9 +371,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -392,7 +408,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,7 +443,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -600,30 +616,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="10" max="10" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="3.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.5703125" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" customWidth="1"/>
-    <col min="26" max="26" width="89.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="10" max="10" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="3.44140625" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5546875" customWidth="1"/>
+    <col min="17" max="17" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5546875" customWidth="1"/>
+    <col min="19" max="19" width="9.44140625" customWidth="1"/>
+    <col min="26" max="26" width="45.33203125" customWidth="1"/>
+    <col min="27" max="27" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,14 +702,8 @@
         <v>16</v>
       </c>
       <c r="U1" s="6"/>
-      <c r="Z1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>31</v>
       </c>
@@ -726,14 +737,14 @@
       <c r="T2">
         <v>1</v>
       </c>
-      <c r="Z2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>41</v>
+      <c r="Z2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>2</v>
       </c>
@@ -761,8 +772,11 @@
       <c r="T3">
         <v>2</v>
       </c>
+      <c r="Z3" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>3</v>
       </c>
@@ -790,11 +804,11 @@
       <c r="T4">
         <v>3</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Z4" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>4</v>
       </c>
@@ -825,7 +839,7 @@
       <c r="T5">
         <v>4</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="Z5" s="8" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>